<commit_message>
add clone and pull
</commit_message>
<xml_diff>
--- a/git_note.xlsx
+++ b/git_note.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
   <si>
     <t>命令</t>
   </si>
@@ -24,6 +24,9 @@
     <t>解释</t>
   </si>
   <si>
+    <t>备注</t>
+  </si>
+  <si>
     <t>git init</t>
   </si>
   <si>
@@ -58,6 +61,12 @@
   </si>
   <si>
     <t>查看git日志</t>
+  </si>
+  <si>
+    <t>git log --pretty=oneline</t>
+  </si>
+  <si>
+    <t>git日志更简洁的显示</t>
   </si>
   <si>
     <t>git reset --hard HEAD^</t>
@@ -73,6 +82,88 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>LLSnoopy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>learngit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.git</t>
+    </r>
+  </si>
+  <si>
+    <t>关联github账户</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>$ git push</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> -u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> origin master</t>
+    </r>
+  </si>
+  <si>
+    <t>第一次推送</t>
+  </si>
+  <si>
+    <t>git push origin master</t>
+  </si>
+  <si>
+    <t>推送到github关联的账户上</t>
+  </si>
+  <si>
+    <r>
+      <t>$ git clone git@github.com:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>LLSnoopy</t>
@@ -83,41 +174,36 @@
         <color theme="1"/>
         <charset val="134"/>
       </rPr>
-      <t>/learngit.git</t>
-    </r>
-  </si>
-  <si>
-    <t>关联github账户</t>
-  </si>
-  <si>
-    <r>
-      <t>$ git push</t>
+      <t>/</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> -u</t>
+      <t>gitskills</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> origin master</t>
+      <t>.git</t>
     </r>
   </si>
   <si>
-    <t>第一次推送</t>
-  </si>
-  <si>
-    <t>git push origin master</t>
-  </si>
-  <si>
-    <t>推送到github关联的账户上</t>
+    <t>从远程库clone到本地</t>
+  </si>
+  <si>
+    <t>本地没有库的时候clone，有库之后用pull</t>
+  </si>
+  <si>
+    <t>git pull origin</t>
+  </si>
+  <si>
+    <t>clone之后再次更新合并</t>
   </si>
 </sst>
 </file>
@@ -126,16 +212,23 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -200,13 +293,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -261,6 +347,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
@@ -269,22 +370,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -299,97 +403,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -401,7 +529,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,6 +541,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -425,61 +565,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,10 +702,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -610,16 +714,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -628,55 +732,55 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -685,62 +789,62 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -748,9 +852,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1097,104 +1210,135 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="37.375" customWidth="1"/>
+    <col min="1" max="1" width="39.125" customWidth="1"/>
     <col min="2" max="2" width="42.5" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="8" ht="27" spans="1:2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" ht="27" spans="1:2">
-      <c r="A9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
-        <v>18</v>
+    <row r="10" ht="27" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>20</v>
+      <c r="A11" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" ht="40.5" spans="1:3">
+      <c r="A15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>